<commit_message>
Integrations : Code pushed with inbound process
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Client/SGBInbound.xlsx
+++ b/src/test/resources/testdata/Client/SGBInbound.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\eApp\src\test\resources\testdata\Client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF45656-55D1-4EBB-BDA7-01578E2A221C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D69FB50-64E7-4641-A66E-2DE37B006CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="731" xr2:uid="{8D0F94DE-3100-47E5-A17C-DB8B711FEBE7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="731" xr2:uid="{8D0F94DE-3100-47E5-A17C-DB8B711FEBE7}"/>
   </bookViews>
   <sheets>
     <sheet name="E-App Wizard Spec" sheetId="34" r:id="rId1"/>
@@ -3622,11 +3622,11 @@
     <t>SmokerStat</t>
   </si>
   <si>
-    <t>1. If (//Holding/Policy/ProductCode = 24 OR //Holding/Policy/ProductCode = 29 OR //Holding/Policy/ProductCode = 30) and (//Holding/Policy/Life/Coverage/LifeParticipant/UnderwritingClass = 1 OR //Holding/Policy/Life/Coverage/LifeParticipant/UnderwritingClass = 2) then verify Attribute //Holding/Policy/Life/Coverage/LifeParticipant/SmokerStat/tc</t>
-  </si>
-  <si>
     <t>1. If //Party/Person/DOBEstimated=False then verify Format //Party/Person/BirthDate = yyyy-MM-dd 
 2. If //Party/Person/DOBEstimated=True then verify Format //Party/Person/BirthDate = yyyy</t>
+  </si>
+  <si>
+    <t>1. If (//Holding/Policy/ProductCode = 2 OR //Holding/Policy/ProductCode = 29 OR //Holding/Policy/ProductCode = 30) and (//Holding/Policy/Life/Coverage/LifeParticipant/UnderwritingClass = 1 OR //Holding/Policy/Life/Coverage/LifeParticipant/UnderwritingClass = 2) then verify Attribute //Holding/Policy/Life/Coverage/LifeParticipant/SmokerStat/tc</t>
   </si>
 </sst>
 </file>
@@ -5318,63 +5318,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C621C402-B2C8-40EA-BB1E-33FF49755F07}">
   <dimension ref="A1:AX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="104.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="104.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="77" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="77" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" style="77" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="77" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="77" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="77" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="77" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" style="77" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" style="77" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.44140625" style="77" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="77" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" style="77" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" style="77" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="77" customWidth="1"/>
     <col min="8" max="8" width="19" style="77" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" style="77" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" style="77" customWidth="1"/>
     <col min="10" max="10" width="17" style="77" customWidth="1"/>
-    <col min="11" max="11" width="37.140625" style="77" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" style="77" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" style="77" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" style="77" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" style="77" customWidth="1"/>
-    <col min="16" max="16" width="22.7109375" style="77" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="25.28515625" style="77" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="18.140625" style="77" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" style="77" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="25.85546875" style="77" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" style="77" customWidth="1"/>
-    <col min="22" max="25" width="19.140625" style="77" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="37.109375" style="77" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="77" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" style="77" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" style="77" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" style="77" customWidth="1"/>
+    <col min="16" max="16" width="22.6640625" style="77" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="25.33203125" style="77" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="18.109375" style="77" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" style="77" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="25.88671875" style="77" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" style="77" customWidth="1"/>
+    <col min="22" max="25" width="19.109375" style="77" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="22" style="77" customWidth="1"/>
-    <col min="27" max="27" width="21.42578125" style="77" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.44140625" style="77" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="3" style="77" customWidth="1"/>
-    <col min="29" max="30" width="3.28515625" style="77" customWidth="1"/>
-    <col min="31" max="31" width="25.85546875" style="73" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.140625" style="77" customWidth="1"/>
-    <col min="33" max="33" width="25.140625" style="77" customWidth="1"/>
-    <col min="34" max="34" width="67.140625" style="151" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="83.85546875" style="77" customWidth="1"/>
-    <col min="36" max="36" width="8.28515625" style="77" customWidth="1"/>
-    <col min="37" max="37" width="8.140625" style="77" customWidth="1"/>
-    <col min="38" max="38" width="9.140625" style="77" customWidth="1"/>
-    <col min="39" max="40" width="8.42578125" style="77" customWidth="1"/>
-    <col min="41" max="41" width="9.42578125" style="77" customWidth="1"/>
-    <col min="42" max="42" width="40.85546875" style="77" customWidth="1"/>
-    <col min="43" max="43" width="7.5703125" style="77" customWidth="1"/>
-    <col min="44" max="44" width="5.140625" style="77" customWidth="1"/>
-    <col min="45" max="45" width="51.28515625" style="77" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="96.28515625" style="77" customWidth="1"/>
-    <col min="47" max="47" width="19.85546875" style="77" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="23.85546875" style="77" customWidth="1"/>
-    <col min="49" max="49" width="18.42578125" style="77" customWidth="1"/>
-    <col min="50" max="50" width="41.85546875" style="77" customWidth="1"/>
-    <col min="51" max="16384" width="9.140625" style="77"/>
+    <col min="29" max="30" width="3.33203125" style="77" customWidth="1"/>
+    <col min="31" max="31" width="25.88671875" style="73" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.109375" style="77" customWidth="1"/>
+    <col min="33" max="33" width="25.109375" style="77" customWidth="1"/>
+    <col min="34" max="34" width="67.109375" style="151" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="83.88671875" style="77" customWidth="1"/>
+    <col min="36" max="36" width="8.33203125" style="77" customWidth="1"/>
+    <col min="37" max="37" width="8.109375" style="77" customWidth="1"/>
+    <col min="38" max="38" width="9.109375" style="77" customWidth="1"/>
+    <col min="39" max="40" width="8.44140625" style="77" customWidth="1"/>
+    <col min="41" max="41" width="9.44140625" style="77" customWidth="1"/>
+    <col min="42" max="42" width="40.88671875" style="77" customWidth="1"/>
+    <col min="43" max="43" width="7.5546875" style="77" customWidth="1"/>
+    <col min="44" max="44" width="5.109375" style="77" customWidth="1"/>
+    <col min="45" max="45" width="51.33203125" style="77" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="96.33203125" style="77" customWidth="1"/>
+    <col min="47" max="47" width="19.88671875" style="77" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="23.88671875" style="77" customWidth="1"/>
+    <col min="49" max="49" width="18.44140625" style="77" customWidth="1"/>
+    <col min="50" max="50" width="41.88671875" style="77" customWidth="1"/>
+    <col min="51" max="16384" width="9.109375" style="77"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="152" t="s">
         <v>5</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
         <v>423</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="3" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
         <v>423</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="4" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="168" t="s">
         <v>423</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="5" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="168" t="s">
         <v>423</v>
       </c>
@@ -5660,7 +5660,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="6" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="168" t="s">
         <v>423</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="7" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="168" t="s">
         <v>423</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>452</v>
       </c>
       <c r="AH7" s="73" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AS7" s="77" t="s">
         <v>460</v>
@@ -5718,7 +5718,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="8" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="168" t="s">
         <v>423</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="9" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="168" t="s">
         <v>423</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="10" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="168" t="s">
         <v>423</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="11" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="168" t="s">
         <v>423</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="12" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="168" t="s">
         <v>423</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>462</v>
       </c>
       <c r="AH12" s="73" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AT12" s="73" t="s">
         <v>432</v>
@@ -5884,16 +5884,16 @@
       <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="143" t="s">
         <v>226</v>
       </c>
@@ -5910,22 +5910,22 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C2" s="146" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C3" s="146" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C4" s="146" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="117" t="s">
         <v>174</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
         <v>176</v>
       </c>
@@ -5959,25 +5959,25 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="147"/>
       <c r="C7" s="146" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="147"/>
       <c r="C8" s="146" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="147"/>
       <c r="C9" s="146" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="77" t="s">
         <v>180</v>
       </c>
@@ -5994,7 +5994,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="77" t="s">
         <v>182</v>
       </c>
@@ -6011,7 +6011,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="77" t="s">
         <v>184</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="77" t="s">
         <v>185</v>
       </c>
@@ -6045,31 +6045,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="147"/>
       <c r="C14" s="146" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="147"/>
       <c r="C15" s="146" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="147"/>
       <c r="C16" s="146" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="147"/>
       <c r="C17" s="146" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="77" t="s">
         <v>186</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="77" t="s">
         <v>188</v>
       </c>
@@ -6100,7 +6100,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="77" t="s">
         <v>190</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="77" t="s">
         <v>192</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="77" t="s">
         <v>194</v>
       </c>
@@ -6151,7 +6151,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="77" t="s">
         <v>196</v>
       </c>
@@ -6168,35 +6168,35 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="146" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="146" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="147"/>
       <c r="C26" s="146" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="147"/>
       <c r="C27" s="146" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="147"/>
       <c r="C28" s="146" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" s="68" t="s">
         <v>231</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="148" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="148" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="149" t="s">
         <v>232</v>
       </c>
@@ -6222,31 +6222,31 @@
         <v>234</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="147"/>
       <c r="C31" s="146" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="147"/>
       <c r="C32" s="146" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="147"/>
       <c r="C33" s="146" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="147"/>
       <c r="C34" s="146" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="77" t="s">
         <v>93</v>
       </c>
@@ -6267,7 +6267,7 @@
       </c>
       <c r="J35" s="142"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="77" t="s">
         <v>202</v>
       </c>
@@ -6284,7 +6284,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="77" t="s">
         <v>173</v>
       </c>
@@ -6301,7 +6301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="77" t="s">
         <v>205</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="77" t="s">
         <v>206</v>
       </c>
@@ -6335,7 +6335,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="77" t="s">
         <v>209</v>
       </c>
@@ -6352,27 +6352,27 @@
         <v>237</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="146" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C42" s="146" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C43" s="146" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C44" s="146" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="77" t="s">
         <v>172</v>
       </c>
@@ -6389,37 +6389,37 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="146" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="146" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="146" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="49" spans="3:3" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C49" s="146" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="50" spans="3:3" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="146" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="51" spans="3:3" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="146" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="52" spans="3:3" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" s="145" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C52" s="146" t="s">
         <v>217</v>
       </c>
@@ -6437,48 +6437,48 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="24" width="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.140625" customWidth="1"/>
-    <col min="27" max="27" width="3.85546875" customWidth="1"/>
-    <col min="28" max="28" width="3.5703125" customWidth="1"/>
-    <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.109375" customWidth="1"/>
+    <col min="27" max="27" width="3.88671875" customWidth="1"/>
+    <col min="28" max="28" width="3.5546875" customWidth="1"/>
+    <col min="29" max="29" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="52" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="66.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="66.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="32" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="44" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="52" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="44" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="52" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:270" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:270" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A1" s="46"/>
       <c r="B1" s="47"/>
       <c r="C1" s="29" t="s">
@@ -6548,7 +6548,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="2" spans="1:270" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:270" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A2" s="46"/>
       <c r="B2" s="47"/>
       <c r="C2" s="29"/>
@@ -6573,7 +6573,7 @@
       <c r="W2" s="31"/>
       <c r="X2" s="31"/>
     </row>
-    <row r="3" spans="1:270" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:270" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="53" t="s">
         <v>239</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:270" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:270" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="95" t="s">
         <v>5</v>
       </c>
@@ -6808,7 +6808,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:270" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:270" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="141" t="s">
         <v>253</v>
       </c>
@@ -6913,7 +6913,7 @@
       <c r="AZ5" s="77"/>
       <c r="BA5" s="77"/>
     </row>
-    <row r="6" spans="1:270" s="69" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:270" s="69" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="141" t="s">
         <v>253</v>
       </c>
@@ -6996,7 +6996,7 @@
       <c r="AZ6" s="140"/>
       <c r="BA6" s="140"/>
     </row>
-    <row r="7" spans="1:270" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:270" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="141" t="s">
         <v>253</v>
       </c>
@@ -7101,7 +7101,7 @@
       <c r="AZ7" s="77"/>
       <c r="BA7" s="77"/>
     </row>
-    <row r="8" spans="1:270" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:270" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="141" t="s">
         <v>253</v>
       </c>
@@ -7206,7 +7206,7 @@
       <c r="AZ8" s="77"/>
       <c r="BA8" s="77"/>
     </row>
-    <row r="9" spans="1:270" s="128" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:270" s="128" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="141" t="s">
         <v>253</v>
       </c>
@@ -7542,7 +7542,7 @@
       <c r="JI9"/>
       <c r="JJ9"/>
     </row>
-    <row r="10" spans="1:270" s="128" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:270" s="128" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="141" t="s">
         <v>253</v>
       </c>
@@ -7878,7 +7878,7 @@
       <c r="JI10"/>
       <c r="JJ10"/>
     </row>
-    <row r="11" spans="1:270" s="128" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:270" s="128" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="141" t="s">
         <v>253</v>
       </c>
@@ -8214,7 +8214,7 @@
       <c r="JI11"/>
       <c r="JJ11"/>
     </row>
-    <row r="12" spans="1:270" s="128" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:270" s="128" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="141" t="s">
         <v>253</v>
       </c>
@@ -8548,7 +8548,7 @@
       <c r="JI12"/>
       <c r="JJ12"/>
     </row>
-    <row r="13" spans="1:270" s="128" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:270" s="128" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="141" t="s">
         <v>253</v>
       </c>
@@ -8888,7 +8888,7 @@
       <c r="JI13"/>
       <c r="JJ13"/>
     </row>
-    <row r="14" spans="1:270" s="128" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:270" s="128" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14" s="141" t="s">
         <v>253</v>
       </c>
@@ -9228,7 +9228,7 @@
       <c r="JI14"/>
       <c r="JJ14"/>
     </row>
-    <row r="15" spans="1:270" s="128" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:270" s="128" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="141" t="s">
         <v>253</v>
       </c>
@@ -9560,7 +9560,7 @@
       <c r="JI15"/>
       <c r="JJ15"/>
     </row>
-    <row r="16" spans="1:270" s="128" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:270" s="128" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="141" t="s">
         <v>253</v>
       </c>
@@ -9894,7 +9894,7 @@
       <c r="JI16"/>
       <c r="JJ16"/>
     </row>
-    <row r="17" spans="1:270" s="128" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:270" s="128" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="141" t="s">
         <v>253</v>
       </c>
@@ -10316,18 +10316,18 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" customWidth="1"/>
-    <col min="3" max="3" width="85.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="48.109375" customWidth="1"/>
+    <col min="3" max="3" width="85.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="25.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="63" t="s">
         <v>296</v>
       </c>
@@ -10353,7 +10353,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>303</v>
       </c>
@@ -10364,7 +10364,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>303</v>
       </c>
@@ -10375,7 +10375,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="120" t="s">
         <v>96</v>
       </c>
@@ -10386,7 +10386,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>307</v>
       </c>
@@ -10397,7 +10397,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -10408,7 +10408,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>307</v>
       </c>
@@ -10419,7 +10419,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>307</v>
       </c>
@@ -10430,7 +10430,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>307</v>
       </c>
@@ -10441,7 +10441,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>312</v>
       </c>
@@ -10452,7 +10452,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>312</v>
       </c>
@@ -10463,7 +10463,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>312</v>
       </c>
@@ -10474,7 +10474,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -10485,7 +10485,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="73" t="s">
         <v>317</v>
       </c>
@@ -10493,7 +10493,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -10504,7 +10504,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -10515,7 +10515,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -10524,7 +10524,7 @@
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -10542,7 +10542,7 @@
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -10551,7 +10551,7 @@
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -10562,7 +10562,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -10573,7 +10573,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -10582,7 +10582,7 @@
       </c>
       <c r="C24" s="122"/>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -10591,7 +10591,7 @@
       </c>
       <c r="C25" s="122"/>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -10600,7 +10600,7 @@
       </c>
       <c r="C26" s="122"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -10611,7 +10611,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -10620,7 +10620,7 @@
       </c>
       <c r="C28" s="122"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -10629,7 +10629,7 @@
       </c>
       <c r="C29" s="122"/>
     </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -10638,7 +10638,7 @@
       </c>
       <c r="C30" s="122"/>
     </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -10647,7 +10647,7 @@
       </c>
       <c r="C31" s="122"/>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -10656,7 +10656,7 @@
       </c>
       <c r="C32" s="122"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -10665,7 +10665,7 @@
       </c>
       <c r="C33" s="122"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -10674,7 +10674,7 @@
       </c>
       <c r="C34" s="122"/>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -10683,7 +10683,7 @@
       </c>
       <c r="C35" s="122"/>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>326</v>
       </c>
@@ -10694,7 +10694,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>326</v>
       </c>
@@ -10705,7 +10705,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>326</v>
       </c>
@@ -10716,7 +10716,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>326</v>
       </c>
@@ -10727,7 +10727,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>328</v>
       </c>
@@ -10738,7 +10738,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>328</v>
       </c>
@@ -10749,7 +10749,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>326</v>
       </c>
@@ -10760,7 +10760,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>334</v>
       </c>
@@ -10771,7 +10771,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>334</v>
       </c>
@@ -10782,7 +10782,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>334</v>
       </c>
@@ -10793,7 +10793,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>334</v>
       </c>
@@ -10804,7 +10804,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>334</v>
       </c>
@@ -10831,23 +10831,23 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.5546875" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="24" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="24" customFormat="1" ht="48" x14ac:dyDescent="0.25">
       <c r="A1" s="63" t="s">
         <v>296</v>
       </c>
@@ -10891,7 +10891,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -10902,7 +10902,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -10913,7 +10913,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -10924,7 +10924,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>107</v>
       </c>
@@ -10935,7 +10935,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -10946,7 +10946,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -10957,7 +10957,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -10968,7 +10968,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -10979,7 +10979,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -10990,7 +10990,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -11002,7 +11002,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -11014,7 +11014,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -11026,7 +11026,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -11038,7 +11038,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -11050,7 +11050,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -11062,7 +11062,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>372</v>
       </c>
@@ -11073,7 +11073,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>372</v>
       </c>
@@ -11084,7 +11084,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>375</v>
       </c>
@@ -11095,7 +11095,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>375</v>
       </c>
@@ -11106,7 +11106,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>375</v>
       </c>
@@ -11117,7 +11117,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>375</v>
       </c>
@@ -11128,7 +11128,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>375</v>
       </c>
@@ -11139,7 +11139,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>375</v>
       </c>
@@ -11150,7 +11150,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>375</v>
       </c>
@@ -11161,7 +11161,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>388</v>
       </c>
@@ -11172,7 +11172,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>388</v>
       </c>
@@ -11183,7 +11183,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>388</v>
       </c>
@@ -11194,22 +11194,22 @@
         <v>392</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>388</v>
       </c>
@@ -11228,9 +11228,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:53" s="24" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" s="24" customFormat="1" ht="54.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
       <c r="B1" s="26"/>
       <c r="C1" s="27" t="s">
@@ -11341,7 +11341,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="2" spans="1:53" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A2" s="25"/>
       <c r="B2" s="26"/>
       <c r="C2" s="27"/>
@@ -11384,7 +11384,7 @@
       <c r="AP2" s="25"/>
       <c r="AS2" s="25"/>
     </row>
-    <row r="3" spans="1:53" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>239</v>
       </c>
@@ -11527,7 +11527,7 @@
       <c r="AZ3" s="46"/>
       <c r="BA3" s="46"/>
     </row>
-    <row r="4" spans="1:53" s="24" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" s="24" customFormat="1" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -11696,6 +11696,42 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <TaxCatchAll xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9" xsi:nil="true"/>
+    <Created0 xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Choice_x002d_Test xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <Date xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <ClientNumber xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <PartitionCode xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9">
+      <UserInfo>
+        <DisplayName>Tammy Sunderland</DisplayName>
+        <AccountId>38</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A419301B98B8354A897828D82A6F00F6" ma:contentTypeVersion="34" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20ca8a0c0d59028efd0f33ef93e3a420">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3e08ed28-a208-4db3-90dc-062006ce0c78" xmlns:ns3="7e386c18-d449-4d9a-a5df-f64c6139a3c9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ecc1aa61ba2aa3d92dc6750af3137611" ns2:_="" ns3:_="">
     <xsd:import namespace="3e08ed28-a208-4db3-90dc-062006ce0c78"/>
@@ -12016,57 +12052,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <TaxCatchAll xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9" xsi:nil="true"/>
-    <Created0 xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Choice_x002d_Test xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <Date xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <ClientNumber xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <PartitionCode xmlns="3e08ed28-a208-4db3-90dc-062006ce0c78" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7e386c18-d449-4d9a-a5df-f64c6139a3c9">
-      <UserInfo>
-        <DisplayName>Tammy Sunderland</DisplayName>
-        <AccountId>38</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{827BF9C6-14B5-43FE-98BA-5537952370B8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BEDA91-E434-447E-A9AB-EB3F15901C97}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3e08ed28-a208-4db3-90dc-062006ce0c78"/>
-    <ds:schemaRef ds:uri="7e386c18-d449-4d9a-a5df-f64c6139a3c9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12089,9 +12078,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79BEDA91-E434-447E-A9AB-EB3F15901C97}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{827BF9C6-14B5-43FE-98BA-5537952370B8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3e08ed28-a208-4db3-90dc-062006ce0c78"/>
+    <ds:schemaRef ds:uri="7e386c18-d449-4d9a-a5df-f64c6139a3c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>